<commit_message>
Repeated FB Prophet for commercial 2021, Resampled commercial 2021 for VertexAI AutoML
</commit_message>
<xml_diff>
--- a/PerformanceParametrs.xlsx
+++ b/PerformanceParametrs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nemaaa/github/Research-KalmarEnergy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD10DA78-0FBA-904B-BB30-61B08811042A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F6E6D2-1450-2F40-B5A4-06C155439045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20860" yWindow="5060" windowWidth="28040" windowHeight="17440" xr2:uid="{D956B77F-D08C-174D-836A-79EDBCF441FF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{D956B77F-D08C-174D-836A-79EDBCF441FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Random Forest</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>5.25</t>
+  </si>
+  <si>
+    <t>226.92</t>
+  </si>
+  <si>
+    <t>15.06</t>
+  </si>
+  <si>
+    <t>12.92</t>
+  </si>
+  <si>
+    <t>8.39</t>
   </si>
 </sst>
 </file>
@@ -131,8 +143,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,18 +480,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3572F30C-D99F-9B47-8351-B55FFDAD8BD6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -505,8 +519,11 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -519,8 +536,11 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -533,8 +553,11 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -547,6 +570,16 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>